<commit_message>
Agrego mensaje de que no existe el codigo en el catalogo de la empresa
</commit_message>
<xml_diff>
--- a/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250722.xlsx
+++ b/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250722.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mojado</t>
+          <t>Comido</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>llovio  y se inundo el galpon</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -490,12 +490,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mojado</t>
+          <t>Comido</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>simil 100</t>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>